<commit_message>
Added second test case to the project
</commit_message>
<xml_diff>
--- a/Testing QA/Test Cases And Evidences - MS4.xlsx
+++ b/Testing QA/Test Cases And Evidences - MS4.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\Desktop\crowdar-challenge\Testing QA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\Desktop\crowdar-challenge\qa.automation.framework\Testing QA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A1A09A3-122F-46EA-A609-5BAE66AC6D84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A5D13E-5572-47F0-BCC3-9A6B0818E72A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5190" yWindow="1965" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3315" yWindow="1305" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TCs" sheetId="1" r:id="rId1"/>
@@ -639,15 +639,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -657,11 +652,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -686,7 +676,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -696,7 +694,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1129,7 +1129,7 @@
   <dimension ref="A1:K1003"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1142,17 +1142,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="52"/>
+      <c r="C1" s="48"/>
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="54"/>
+      <c r="C2" s="50"/>
       <c r="J2" s="1"/>
     </row>
     <row r="3" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1188,47 +1188,47 @@
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="2:11" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B8" s="55" t="s">
+      <c r="B8" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="56"/>
+      <c r="C8" s="52"/>
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="57" t="s">
+      <c r="B9" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="58"/>
+      <c r="C9" s="54"/>
       <c r="J9" s="1"/>
     </row>
     <row r="10" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="46" t="s">
+      <c r="B11" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="47" t="s">
+      <c r="C11" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="48" t="s">
+      <c r="D11" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="49"/>
-      <c r="F11" s="50"/>
-      <c r="G11" s="47" t="s">
+      <c r="E11" s="62"/>
+      <c r="F11" s="63"/>
+      <c r="G11" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="H11" s="47" t="s">
+      <c r="H11" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="I11" s="47" t="s">
+      <c r="I11" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="J11" s="47" t="s">
+      <c r="J11" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="K11" s="47" t="s">
+      <c r="K11" s="41" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1239,12 +1239,12 @@
       <c r="C12" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="40" t="s">
+      <c r="D12" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="41"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="59" t="s">
+      <c r="E12" s="56"/>
+      <c r="F12" s="57"/>
+      <c r="G12" s="42" t="s">
         <v>39</v>
       </c>
       <c r="H12" s="39" t="s">
@@ -1265,11 +1265,11 @@
         <v>18</v>
       </c>
       <c r="C13" s="7"/>
-      <c r="D13" s="40" t="s">
+      <c r="D13" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="41"/>
-      <c r="F13" s="42"/>
+      <c r="E13" s="56"/>
+      <c r="F13" s="57"/>
       <c r="G13" s="36"/>
       <c r="H13" s="36"/>
       <c r="I13" s="17"/>
@@ -1281,11 +1281,11 @@
         <v>19</v>
       </c>
       <c r="C14" s="38"/>
-      <c r="D14" s="60" t="s">
+      <c r="D14" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="61"/>
-      <c r="F14" s="62"/>
+      <c r="E14" s="59"/>
+      <c r="F14" s="60"/>
       <c r="G14" s="33"/>
       <c r="H14" s="33"/>
       <c r="I14" s="18"/>
@@ -1299,11 +1299,11 @@
       <c r="C15" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="43" t="s">
+      <c r="D15" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="44"/>
-      <c r="F15" s="45"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="46"/>
       <c r="G15" s="29" t="s">
         <v>40</v>
       </c>
@@ -1325,11 +1325,11 @@
         <v>18</v>
       </c>
       <c r="C16" s="17"/>
-      <c r="D16" s="40" t="s">
+      <c r="D16" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="E16" s="41"/>
-      <c r="F16" s="42"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="57"/>
       <c r="G16" s="17"/>
       <c r="H16" s="17"/>
       <c r="I16" s="17"/>
@@ -1341,11 +1341,11 @@
         <v>19</v>
       </c>
       <c r="C17" s="18"/>
-      <c r="D17" s="60" t="s">
+      <c r="D17" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="E17" s="61"/>
-      <c r="F17" s="62"/>
+      <c r="E17" s="59"/>
+      <c r="F17" s="60"/>
       <c r="G17" s="18"/>
       <c r="H17" s="18"/>
       <c r="I17" s="18"/>
@@ -1359,11 +1359,11 @@
       <c r="C18" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="43" t="s">
+      <c r="D18" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="E18" s="44"/>
-      <c r="F18" s="45"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="46"/>
       <c r="G18" s="29" t="s">
         <v>41</v>
       </c>
@@ -1385,11 +1385,11 @@
         <v>18</v>
       </c>
       <c r="C19" s="17"/>
-      <c r="D19" s="40" t="s">
+      <c r="D19" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="E19" s="41"/>
-      <c r="F19" s="42"/>
+      <c r="E19" s="56"/>
+      <c r="F19" s="57"/>
       <c r="G19" s="17"/>
       <c r="H19" s="17"/>
       <c r="I19" s="17"/>
@@ -1401,11 +1401,11 @@
         <v>19</v>
       </c>
       <c r="C20" s="18"/>
-      <c r="D20" s="60" t="s">
+      <c r="D20" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="E20" s="61"/>
-      <c r="F20" s="62"/>
+      <c r="E20" s="59"/>
+      <c r="F20" s="60"/>
       <c r="G20" s="18"/>
       <c r="H20" s="18"/>
       <c r="I20" s="18"/>
@@ -4127,6 +4127,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D20:F20"/>
     <mergeCell ref="D15:F15"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
@@ -4136,11 +4141,6 @@
     <mergeCell ref="D13:F13"/>
     <mergeCell ref="D14:F14"/>
     <mergeCell ref="D11:F11"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D20:F20"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <conditionalFormatting sqref="J12:J20">
@@ -5015,7 +5015,7 @@
       <c r="V40" s="14"/>
     </row>
     <row r="41" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="D41" s="63" t="s">
+      <c r="D41" s="43" t="s">
         <v>34</v>
       </c>
       <c r="E41" s="5"/>

</xml_diff>

<commit_message>
added third test case
</commit_message>
<xml_diff>
--- a/Testing QA/Test Cases And Evidences - MS4.xlsx
+++ b/Testing QA/Test Cases And Evidences - MS4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\Desktop\crowdar-challenge\qa.automation.framework\Testing QA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A5D13E-5572-47F0-BCC3-9A6B0818E72A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86EAB595-FBE2-4A04-871B-E1973AE2A6C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3315" yWindow="1305" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -165,9 +165,6 @@
     <t>Verify that the validation message is displayed in the case of a blocked-out user login by entering valid credentials and clicking on the 'LOGIN' button.</t>
   </si>
   <si>
-    <t>Verify that the User is not able to log in with a blank Username or Password</t>
-  </si>
-  <si>
     <t>1.- Validate the input box that would say Username is empty</t>
   </si>
   <si>
@@ -180,7 +177,10 @@
     <t>It should show a validation message that would say: "Epic sadface: Sorry, this user has been locked out."</t>
   </si>
   <si>
-    <t>It should show a validation message that would say: "Epic sadface: Username is required"</t>
+    <t>Verify that the User is not able to log in with invalid credentials</t>
+  </si>
+  <si>
+    <t>It should show a validation message that would say: "Epic sadface: Username and password do not match any user in this service"</t>
   </si>
 </sst>
 </file>
@@ -643,6 +643,24 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -674,24 +692,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1128,8 +1128,8 @@
   </sheetPr>
   <dimension ref="A1:K1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1142,17 +1142,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="48"/>
+      <c r="C1" s="54"/>
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="50"/>
+      <c r="C2" s="56"/>
       <c r="J2" s="1"/>
     </row>
     <row r="3" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1188,17 +1188,17 @@
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="2:11" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B8" s="51" t="s">
+      <c r="B8" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="52"/>
+      <c r="C8" s="58"/>
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="53" t="s">
+      <c r="B9" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="54"/>
+      <c r="C9" s="60"/>
       <c r="J9" s="1"/>
     </row>
     <row r="10" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -1239,13 +1239,13 @@
       <c r="C12" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="55" t="s">
+      <c r="D12" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="56"/>
-      <c r="F12" s="57"/>
+      <c r="E12" s="45"/>
+      <c r="F12" s="46"/>
       <c r="G12" s="42" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H12" s="39" t="s">
         <v>14</v>
@@ -1265,11 +1265,11 @@
         <v>18</v>
       </c>
       <c r="C13" s="7"/>
-      <c r="D13" s="55" t="s">
+      <c r="D13" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="56"/>
-      <c r="F13" s="57"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="46"/>
       <c r="G13" s="36"/>
       <c r="H13" s="36"/>
       <c r="I13" s="17"/>
@@ -1281,11 +1281,11 @@
         <v>19</v>
       </c>
       <c r="C14" s="38"/>
-      <c r="D14" s="58" t="s">
+      <c r="D14" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="59"/>
-      <c r="F14" s="60"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="49"/>
       <c r="G14" s="33"/>
       <c r="H14" s="33"/>
       <c r="I14" s="18"/>
@@ -1299,13 +1299,13 @@
       <c r="C15" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="44" t="s">
+      <c r="D15" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="45"/>
-      <c r="F15" s="46"/>
+      <c r="E15" s="51"/>
+      <c r="F15" s="52"/>
       <c r="G15" s="29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H15" s="20" t="s">
         <v>14</v>
@@ -1325,11 +1325,11 @@
         <v>18</v>
       </c>
       <c r="C16" s="17"/>
-      <c r="D16" s="55" t="s">
+      <c r="D16" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="E16" s="56"/>
-      <c r="F16" s="57"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="46"/>
       <c r="G16" s="17"/>
       <c r="H16" s="17"/>
       <c r="I16" s="17"/>
@@ -1341,11 +1341,11 @@
         <v>19</v>
       </c>
       <c r="C17" s="18"/>
-      <c r="D17" s="58" t="s">
+      <c r="D17" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="E17" s="59"/>
-      <c r="F17" s="60"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="49"/>
       <c r="G17" s="18"/>
       <c r="H17" s="18"/>
       <c r="I17" s="18"/>
@@ -1357,13 +1357,13 @@
         <v>26</v>
       </c>
       <c r="C18" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="44" t="s">
-        <v>37</v>
-      </c>
-      <c r="E18" s="45"/>
-      <c r="F18" s="46"/>
+      <c r="E18" s="51"/>
+      <c r="F18" s="52"/>
       <c r="G18" s="29" t="s">
         <v>41</v>
       </c>
@@ -1385,11 +1385,11 @@
         <v>18</v>
       </c>
       <c r="C19" s="17"/>
-      <c r="D19" s="55" t="s">
-        <v>38</v>
+      <c r="D19" s="44" t="s">
+        <v>37</v>
       </c>
-      <c r="E19" s="56"/>
-      <c r="F19" s="57"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="46"/>
       <c r="G19" s="17"/>
       <c r="H19" s="17"/>
       <c r="I19" s="17"/>
@@ -1401,11 +1401,11 @@
         <v>19</v>
       </c>
       <c r="C20" s="18"/>
-      <c r="D20" s="58" t="s">
+      <c r="D20" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="E20" s="59"/>
-      <c r="F20" s="60"/>
+      <c r="E20" s="48"/>
+      <c r="F20" s="49"/>
       <c r="G20" s="18"/>
       <c r="H20" s="18"/>
       <c r="I20" s="18"/>
@@ -4127,11 +4127,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D20:F20"/>
     <mergeCell ref="D15:F15"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
@@ -4141,6 +4136,11 @@
     <mergeCell ref="D13:F13"/>
     <mergeCell ref="D14:F14"/>
     <mergeCell ref="D11:F11"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D20:F20"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <conditionalFormatting sqref="J12:J20">

</xml_diff>

<commit_message>
fixed a problem with an image on the test cases section in the Testing QA directory
</commit_message>
<xml_diff>
--- a/Testing QA/Test Cases And Evidences - MS4.xlsx
+++ b/Testing QA/Test Cases And Evidences - MS4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\Desktop\crowdar-challenge\qa.automation.framework\Testing QA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86EAB595-FBE2-4A04-871B-E1973AE2A6C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D649982B-D32F-4225-B6FE-BCEF4273C8F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3315" yWindow="1305" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TCs" sheetId="1" r:id="rId1"/>
@@ -643,24 +643,6 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -692,6 +674,24 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -875,22 +875,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>191548</xdr:colOff>
-      <xdr:row>78</xdr:row>
-      <xdr:rowOff>76998</xdr:rowOff>
+      <xdr:colOff>353474</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>105571</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Imagen 10">
+        <xdr:cNvPr id="4" name="Imagen 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BAAA82D8-2294-7BD8-E438-E002D7EA7189}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB9FAAEB-C13E-5609-BAC7-4CCD21547C27}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -912,8 +912,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2590800" y="7029450"/>
-          <a:ext cx="7506748" cy="5715798"/>
+          <a:off x="2743200" y="6905625"/>
+          <a:ext cx="7516274" cy="5706271"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1128,7 +1128,7 @@
   </sheetPr>
   <dimension ref="A1:K1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
@@ -1142,17 +1142,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="54"/>
+      <c r="C1" s="48"/>
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="56"/>
+      <c r="C2" s="50"/>
       <c r="J2" s="1"/>
     </row>
     <row r="3" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1188,17 +1188,17 @@
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="2:11" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B8" s="57" t="s">
+      <c r="B8" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="58"/>
+      <c r="C8" s="52"/>
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="59" t="s">
+      <c r="B9" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="60"/>
+      <c r="C9" s="54"/>
       <c r="J9" s="1"/>
     </row>
     <row r="10" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -1239,11 +1239,11 @@
       <c r="C12" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="44" t="s">
+      <c r="D12" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="45"/>
-      <c r="F12" s="46"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="57"/>
       <c r="G12" s="42" t="s">
         <v>38</v>
       </c>
@@ -1265,11 +1265,11 @@
         <v>18</v>
       </c>
       <c r="C13" s="7"/>
-      <c r="D13" s="44" t="s">
+      <c r="D13" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="45"/>
-      <c r="F13" s="46"/>
+      <c r="E13" s="56"/>
+      <c r="F13" s="57"/>
       <c r="G13" s="36"/>
       <c r="H13" s="36"/>
       <c r="I13" s="17"/>
@@ -1281,11 +1281,11 @@
         <v>19</v>
       </c>
       <c r="C14" s="38"/>
-      <c r="D14" s="47" t="s">
+      <c r="D14" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="48"/>
-      <c r="F14" s="49"/>
+      <c r="E14" s="59"/>
+      <c r="F14" s="60"/>
       <c r="G14" s="33"/>
       <c r="H14" s="33"/>
       <c r="I14" s="18"/>
@@ -1299,11 +1299,11 @@
       <c r="C15" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="50" t="s">
+      <c r="D15" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="51"/>
-      <c r="F15" s="52"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="46"/>
       <c r="G15" s="29" t="s">
         <v>39</v>
       </c>
@@ -1325,11 +1325,11 @@
         <v>18</v>
       </c>
       <c r="C16" s="17"/>
-      <c r="D16" s="44" t="s">
+      <c r="D16" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="E16" s="45"/>
-      <c r="F16" s="46"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="57"/>
       <c r="G16" s="17"/>
       <c r="H16" s="17"/>
       <c r="I16" s="17"/>
@@ -1341,11 +1341,11 @@
         <v>19</v>
       </c>
       <c r="C17" s="18"/>
-      <c r="D17" s="47" t="s">
+      <c r="D17" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="E17" s="48"/>
-      <c r="F17" s="49"/>
+      <c r="E17" s="59"/>
+      <c r="F17" s="60"/>
       <c r="G17" s="18"/>
       <c r="H17" s="18"/>
       <c r="I17" s="18"/>
@@ -1359,11 +1359,11 @@
       <c r="C18" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="50" t="s">
+      <c r="D18" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="E18" s="51"/>
-      <c r="F18" s="52"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="46"/>
       <c r="G18" s="29" t="s">
         <v>41</v>
       </c>
@@ -1385,11 +1385,11 @@
         <v>18</v>
       </c>
       <c r="C19" s="17"/>
-      <c r="D19" s="44" t="s">
+      <c r="D19" s="55" t="s">
         <v>37</v>
       </c>
-      <c r="E19" s="45"/>
-      <c r="F19" s="46"/>
+      <c r="E19" s="56"/>
+      <c r="F19" s="57"/>
       <c r="G19" s="17"/>
       <c r="H19" s="17"/>
       <c r="I19" s="17"/>
@@ -1401,11 +1401,11 @@
         <v>19</v>
       </c>
       <c r="C20" s="18"/>
-      <c r="D20" s="47" t="s">
+      <c r="D20" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="E20" s="48"/>
-      <c r="F20" s="49"/>
+      <c r="E20" s="59"/>
+      <c r="F20" s="60"/>
       <c r="G20" s="18"/>
       <c r="H20" s="18"/>
       <c r="I20" s="18"/>
@@ -4127,6 +4127,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D20:F20"/>
     <mergeCell ref="D15:F15"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
@@ -4136,11 +4141,6 @@
     <mergeCell ref="D13:F13"/>
     <mergeCell ref="D14:F14"/>
     <mergeCell ref="D11:F11"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D20:F20"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <conditionalFormatting sqref="J12:J20">
@@ -4188,7 +4188,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B66EAA69-EFCD-45F8-A730-2076085D2977}">
   <dimension ref="B1:V82"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
       <selection activeCell="Q54" sqref="Q54"/>
     </sheetView>
   </sheetViews>

</xml_diff>